<commit_message>
This closes #1296, add new function `GetRowOpts` for stream reader (#1297)
- Support get rows properties by `GetRowOpts` function
- New exported constant `MaxCellStyles`
</commit_message>
<xml_diff>
--- a/test/Book1.xlsx
+++ b/test/Book1.xlsx
@@ -2576,7 +2576,7 @@
     <col customWidth="1" width="0" max="9" min="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25" s="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25" s="2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>